<commit_message>
1 test case is failing
</commit_message>
<xml_diff>
--- a/Project/testdata/data.xlsx
+++ b/Project/testdata/data.xlsx
@@ -695,15 +695,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Gagandeep</v>
+        <v>SK</v>
       </c>
       <c r="B1" t="str">
-        <v>wertykjhgfdaasdfghmkjn@gmail.com</v>
+        <v>RKRS121345678@gmail.cm</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Kanta</v>
+        <v>RS</v>
       </c>
       <c r="B2" t="str">
         <v>Qwertasdf@#$7654</v>

</xml_diff>